<commit_message>
25/4 end of day -> elasticities weekend/day over multiple periods
</commit_message>
<xml_diff>
--- a/Model2/excel/Time_periods.xlsx
+++ b/Model2/excel/Time_periods.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Include?</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>Period</t>
   </si>
 </sst>
 </file>
@@ -453,20 +459,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -474,35 +480,51 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>6721</v>
+        <v>2689</v>
       </c>
       <c r="B4">
-        <v>52.142857142857146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26.071428571428573</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5545</v>
+      </c>
+      <c r="B5">
+        <v>26.071428571428573</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
@@ -513,34 +535,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:X94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:M4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15:X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1177</v>
       </c>
@@ -550,26 +578,37 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>6721</v>
       </c>
-      <c r="F4">
+      <c r="K4">
         <v>52.142857142857103</v>
       </c>
-      <c r="H4">
+      <c r="M4">
         <v>1177</v>
       </c>
-      <c r="I4">
+      <c r="N4">
         <v>3.480072593</v>
       </c>
-      <c r="L4">
+      <c r="Q4">
         <v>6721</v>
       </c>
-      <c r="M4">
+      <c r="R4">
         <v>52.142857142857146</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <f>R4/3</f>
+        <v>17.380952380952383</v>
+      </c>
+      <c r="V4">
+        <f>R4/2</f>
+        <v>26.071428571428573</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2185</v>
       </c>
@@ -579,21 +618,24 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="J5">
         <v>6745</v>
       </c>
-      <c r="F5">
+      <c r="K5">
         <v>52.142857142857146</v>
       </c>
-      <c r="H5">
-        <f t="shared" ref="H5:H10" si="0">H4+24</f>
+      <c r="M5">
+        <f t="shared" ref="M5:M10" si="0">M4+24</f>
         <v>1201</v>
       </c>
-      <c r="I5">
+      <c r="N5">
         <v>3.480072593</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2689</v>
       </c>
@@ -601,23 +643,26 @@
         <v>5.4874150473299999</v>
       </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="J6">
         <v>6769</v>
       </c>
-      <c r="F6">
+      <c r="K6">
         <v>52.142857142857146</v>
       </c>
-      <c r="H6">
+      <c r="M6">
         <f t="shared" si="0"/>
         <v>1225</v>
       </c>
-      <c r="I6">
+      <c r="N6">
         <v>3.480072593</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3697</v>
       </c>
@@ -625,23 +670,32 @@
         <v>2.5018135322499999</v>
       </c>
       <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="E7">
+      <c r="J7">
         <v>6793</v>
       </c>
-      <c r="F7">
+      <c r="K7">
         <v>52.142857142857146</v>
       </c>
-      <c r="H7">
+      <c r="M7">
         <f t="shared" si="0"/>
         <v>1249</v>
       </c>
-      <c r="I7">
+      <c r="N7">
         <v>3.480072593</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3865</v>
       </c>
@@ -649,23 +703,38 @@
         <v>2.6593111184499998</v>
       </c>
       <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="J8">
         <v>6817</v>
       </c>
-      <c r="F8">
+      <c r="K8">
         <v>52.142857142857146</v>
       </c>
-      <c r="H8">
+      <c r="M8">
         <f t="shared" si="0"/>
         <v>1273</v>
       </c>
-      <c r="I8">
+      <c r="N8">
         <v>3.480072593</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>2689</v>
+      </c>
+      <c r="V8">
+        <v>17.380952380952383</v>
+      </c>
+      <c r="W8">
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4705</v>
       </c>
@@ -673,23 +742,38 @@
         <v>1.2990251051499999</v>
       </c>
       <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>6</v>
       </c>
-      <c r="E9">
+      <c r="J9">
         <v>6841</v>
       </c>
-      <c r="F9">
+      <c r="K9">
         <v>52.142857142857146</v>
       </c>
-      <c r="H9">
+      <c r="M9">
         <f t="shared" si="0"/>
         <v>1297</v>
       </c>
-      <c r="I9">
+      <c r="N9">
         <v>3.480072593</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>5545</v>
+      </c>
+      <c r="V9">
+        <v>17.380952380952383</v>
+      </c>
+      <c r="W9">
+        <v>3</v>
+      </c>
+      <c r="X9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5209</v>
       </c>
@@ -697,23 +781,38 @@
         <v>5.7625265071099996</v>
       </c>
       <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
         <v>7</v>
       </c>
-      <c r="E10">
+      <c r="J10">
         <v>6865</v>
       </c>
-      <c r="F10">
+      <c r="K10">
         <v>52.142857142857146</v>
       </c>
-      <c r="H10">
+      <c r="M10">
         <f t="shared" si="0"/>
         <v>1321</v>
       </c>
-      <c r="I10">
+      <c r="N10">
         <v>3.480072593</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>8065</v>
+      </c>
+      <c r="V10">
+        <v>17.380952380952383</v>
+      </c>
+      <c r="W10">
+        <v>4</v>
+      </c>
+      <c r="X10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5545</v>
       </c>
@@ -721,16 +820,19 @@
         <v>5.8162463790599999</v>
       </c>
       <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
         <v>8</v>
       </c>
-      <c r="H11">
+      <c r="M11">
         <v>2185</v>
       </c>
-      <c r="I11">
+      <c r="N11">
         <v>4.3355659820000003</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6721</v>
       </c>
@@ -738,17 +840,20 @@
         <v>2.3624937309799998</v>
       </c>
       <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
         <v>9</v>
       </c>
-      <c r="H12">
-        <f t="shared" ref="H12:H17" si="1">H11+24</f>
+      <c r="M12">
+        <f t="shared" ref="M12:M17" si="1">M11+24</f>
         <v>2209</v>
       </c>
-      <c r="I12">
+      <c r="N12">
         <v>4.3355659820000003</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7225</v>
       </c>
@@ -756,17 +861,20 @@
         <v>4.7326870781299997</v>
       </c>
       <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
         <v>10</v>
       </c>
-      <c r="H13">
+      <c r="M13">
         <f t="shared" si="1"/>
         <v>2233</v>
       </c>
-      <c r="I13">
+      <c r="N13">
         <v>4.3355659820000003</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7897</v>
       </c>
@@ -774,17 +882,20 @@
         <v>4.6046707498900004</v>
       </c>
       <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
         <v>11</v>
       </c>
-      <c r="H14">
+      <c r="M14">
         <f t="shared" si="1"/>
         <v>2257</v>
       </c>
-      <c r="I14">
+      <c r="N14">
         <v>4.3355659820000003</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8065</v>
       </c>
@@ -792,17 +903,32 @@
         <v>6.1457110019499996</v>
       </c>
       <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
         <v>12</v>
       </c>
-      <c r="H15">
+      <c r="M15">
         <f t="shared" si="1"/>
         <v>2281</v>
       </c>
-      <c r="I15">
+      <c r="N15">
         <v>4.3355659820000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>2689</v>
+      </c>
+      <c r="V15">
+        <v>26.071428571428573</v>
+      </c>
+      <c r="W15">
+        <v>2</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8401</v>
       </c>
@@ -810,702 +936,717 @@
         <v>2.9553183178400002</v>
       </c>
       <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
         <v>13</v>
       </c>
-      <c r="H16">
+      <c r="M16">
         <f t="shared" si="1"/>
         <v>2305</v>
       </c>
-      <c r="I16">
+      <c r="N16">
         <v>4.3355659820000003</v>
       </c>
-    </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H17">
+      <c r="U16">
+        <v>5545</v>
+      </c>
+      <c r="V16">
+        <v>26.071428571428573</v>
+      </c>
+      <c r="W16">
+        <v>3</v>
+      </c>
+      <c r="X16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M17">
         <f t="shared" si="1"/>
         <v>2329</v>
       </c>
-      <c r="I17">
+      <c r="N17">
         <v>4.3355659820000003</v>
       </c>
     </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H18">
+    <row r="18" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M18">
         <v>2689</v>
       </c>
-      <c r="I18">
+      <c r="N18">
         <v>5.4874150469999998</v>
       </c>
     </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H19">
-        <f t="shared" ref="H19:H24" si="2">H18+24</f>
+    <row r="19" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <f t="shared" ref="M19:M24" si="2">M18+24</f>
         <v>2713</v>
       </c>
-      <c r="I19">
+      <c r="N19">
         <v>5.4874150469999998</v>
       </c>
     </row>
-    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H20">
+    <row r="20" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M20">
         <f t="shared" si="2"/>
         <v>2737</v>
       </c>
-      <c r="I20">
+      <c r="N20">
         <v>5.4874150469999998</v>
       </c>
     </row>
-    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H21">
+    <row r="21" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M21">
         <f t="shared" si="2"/>
         <v>2761</v>
       </c>
-      <c r="I21">
+      <c r="N21">
         <v>5.4874150469999998</v>
       </c>
     </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H22">
+    <row r="22" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M22">
         <f t="shared" si="2"/>
         <v>2785</v>
       </c>
-      <c r="I22">
+      <c r="N22">
         <v>5.4874150469999998</v>
       </c>
     </row>
-    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H23">
+    <row r="23" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M23">
         <f t="shared" si="2"/>
         <v>2809</v>
       </c>
-      <c r="I23">
+      <c r="N23">
         <v>5.4874150469999998</v>
       </c>
     </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H24">
+    <row r="24" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M24">
         <f t="shared" si="2"/>
         <v>2833</v>
       </c>
-      <c r="I24">
+      <c r="N24">
         <v>5.4874150469999998</v>
       </c>
     </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H25">
+    <row r="25" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M25">
         <v>3697</v>
       </c>
-      <c r="I25">
+      <c r="N25">
         <v>2.5018135319999999</v>
       </c>
     </row>
-    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H26">
-        <f t="shared" ref="H26:H31" si="3">H25+24</f>
+    <row r="26" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <f t="shared" ref="M26:M31" si="3">M25+24</f>
         <v>3721</v>
       </c>
-      <c r="I26">
+      <c r="N26">
         <v>2.5018135319999999</v>
       </c>
     </row>
-    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H27">
+    <row r="27" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M27">
         <f t="shared" si="3"/>
         <v>3745</v>
       </c>
-      <c r="I27">
+      <c r="N27">
         <v>2.5018135319999999</v>
       </c>
     </row>
-    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H28">
+    <row r="28" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M28">
         <f t="shared" si="3"/>
         <v>3769</v>
       </c>
-      <c r="I28">
+      <c r="N28">
         <v>2.5018135319999999</v>
       </c>
     </row>
-    <row r="29" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H29">
+    <row r="29" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M29">
         <f t="shared" si="3"/>
         <v>3793</v>
       </c>
-      <c r="I29">
+      <c r="N29">
         <v>2.5018135319999999</v>
       </c>
     </row>
-    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H30">
+    <row r="30" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M30">
         <f t="shared" si="3"/>
         <v>3817</v>
       </c>
-      <c r="I30">
+      <c r="N30">
         <v>2.5018135319999999</v>
       </c>
     </row>
-    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H31">
+    <row r="31" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M31">
         <f t="shared" si="3"/>
         <v>3841</v>
       </c>
-      <c r="I31">
+      <c r="N31">
         <v>2.5018135319999999</v>
       </c>
-      <c r="N31">
+      <c r="S31">
         <f>365*24/(168*13)</f>
         <v>4.0109890109890109</v>
       </c>
     </row>
-    <row r="32" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H32">
+    <row r="32" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M32">
         <v>3865</v>
       </c>
-      <c r="I32">
+      <c r="N32">
         <v>2.6593111180000002</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H33">
-        <f t="shared" ref="H33:H38" si="4">H32+24</f>
+    <row r="33" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <f t="shared" ref="M33:M38" si="4">M32+24</f>
         <v>3889</v>
       </c>
-      <c r="I33">
+      <c r="N33">
         <v>2.6593111180000002</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H34">
+    <row r="34" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M34">
         <f t="shared" si="4"/>
         <v>3913</v>
       </c>
-      <c r="I34">
+      <c r="N34">
         <v>2.6593111180000002</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H35">
+    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M35">
         <f t="shared" si="4"/>
         <v>3937</v>
       </c>
-      <c r="I35">
+      <c r="N35">
         <v>2.6593111180000002</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H36">
+    <row r="36" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M36">
         <f t="shared" si="4"/>
         <v>3961</v>
       </c>
-      <c r="I36">
+      <c r="N36">
         <v>2.6593111180000002</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H37">
+    <row r="37" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M37">
         <f t="shared" si="4"/>
         <v>3985</v>
       </c>
-      <c r="I37">
+      <c r="N37">
         <v>2.6593111180000002</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H38">
+    <row r="38" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M38">
         <f t="shared" si="4"/>
         <v>4009</v>
       </c>
-      <c r="I38">
+      <c r="N38">
         <v>2.6593111180000002</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H39">
+    <row r="39" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M39">
         <v>4705</v>
       </c>
-      <c r="I39">
+      <c r="N39">
         <v>1.2990251049999999</v>
       </c>
     </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H40">
-        <f t="shared" ref="H40:H45" si="5">H39+24</f>
+    <row r="40" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <f t="shared" ref="M40:M45" si="5">M39+24</f>
         <v>4729</v>
       </c>
-      <c r="I40">
+      <c r="N40">
         <v>1.2990251049999999</v>
       </c>
     </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H41">
+    <row r="41" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M41">
         <f t="shared" si="5"/>
         <v>4753</v>
       </c>
-      <c r="I41">
+      <c r="N41">
         <v>1.2990251049999999</v>
       </c>
     </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H42">
+    <row r="42" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M42">
         <f t="shared" si="5"/>
         <v>4777</v>
       </c>
-      <c r="I42">
+      <c r="N42">
         <v>1.2990251049999999</v>
       </c>
     </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H43">
+    <row r="43" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M43">
         <f t="shared" si="5"/>
         <v>4801</v>
       </c>
-      <c r="I43">
+      <c r="N43">
         <v>1.2990251049999999</v>
       </c>
     </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H44">
+    <row r="44" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M44">
         <f t="shared" si="5"/>
         <v>4825</v>
       </c>
-      <c r="I44">
+      <c r="N44">
         <v>1.2990251049999999</v>
       </c>
     </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H45">
+    <row r="45" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M45">
         <f t="shared" si="5"/>
         <v>4849</v>
       </c>
-      <c r="I45">
+      <c r="N45">
         <v>1.2990251049999999</v>
       </c>
     </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H46">
+    <row r="46" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M46">
         <v>5209</v>
       </c>
-      <c r="I46">
+      <c r="N46">
         <v>5.7625265069999996</v>
       </c>
     </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H47">
-        <f t="shared" ref="H47:H52" si="6">H46+24</f>
+    <row r="47" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <f t="shared" ref="M47:M52" si="6">M46+24</f>
         <v>5233</v>
       </c>
-      <c r="I47">
+      <c r="N47">
         <v>5.7625265069999996</v>
       </c>
     </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H48">
+    <row r="48" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M48">
         <f t="shared" si="6"/>
         <v>5257</v>
       </c>
-      <c r="I48">
+      <c r="N48">
         <v>5.7625265069999996</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H49">
+    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M49">
         <f t="shared" si="6"/>
         <v>5281</v>
       </c>
-      <c r="I49">
+      <c r="N49">
         <v>5.7625265069999996</v>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H50">
+    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M50">
         <f t="shared" si="6"/>
         <v>5305</v>
       </c>
-      <c r="I50">
+      <c r="N50">
         <v>5.7625265069999996</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H51">
+    <row r="51" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M51">
         <f t="shared" si="6"/>
         <v>5329</v>
       </c>
-      <c r="I51">
+      <c r="N51">
         <v>5.7625265069999996</v>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H52">
+    <row r="52" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M52">
         <f t="shared" si="6"/>
         <v>5353</v>
       </c>
-      <c r="I52">
+      <c r="N52">
         <v>5.7625265069999996</v>
       </c>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H53">
+    <row r="53" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M53">
         <v>5545</v>
       </c>
-      <c r="I53">
+      <c r="N53">
         <v>5.8162463789999999</v>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H54">
-        <f t="shared" ref="H54:H59" si="7">H53+24</f>
+    <row r="54" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M54">
+        <f t="shared" ref="M54:M59" si="7">M53+24</f>
         <v>5569</v>
       </c>
-      <c r="I54">
+      <c r="N54">
         <v>5.8162463789999999</v>
       </c>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H55">
+    <row r="55" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M55">
         <f t="shared" si="7"/>
         <v>5593</v>
       </c>
-      <c r="I55">
+      <c r="N55">
         <v>5.8162463789999999</v>
       </c>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H56">
+    <row r="56" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M56">
         <f t="shared" si="7"/>
         <v>5617</v>
       </c>
-      <c r="I56">
+      <c r="N56">
         <v>5.8162463789999999</v>
       </c>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H57">
+    <row r="57" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M57">
         <f t="shared" si="7"/>
         <v>5641</v>
       </c>
-      <c r="I57">
+      <c r="N57">
         <v>5.8162463789999999</v>
       </c>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H58">
+    <row r="58" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M58">
         <f t="shared" si="7"/>
         <v>5665</v>
       </c>
-      <c r="I58">
+      <c r="N58">
         <v>5.8162463789999999</v>
       </c>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H59">
+    <row r="59" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M59">
         <f t="shared" si="7"/>
         <v>5689</v>
       </c>
-      <c r="I59">
+      <c r="N59">
         <v>5.8162463789999999</v>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H60">
+    <row r="60" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M60">
         <v>6721</v>
       </c>
-      <c r="I60">
+      <c r="N60">
         <v>52.142857142857146</v>
       </c>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H61">
+    <row r="61" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M61">
         <v>6745</v>
       </c>
-      <c r="I61">
+      <c r="N61">
         <v>52.142857142857146</v>
       </c>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H62">
+    <row r="62" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M62">
         <v>6769</v>
       </c>
-      <c r="I62">
+      <c r="N62">
         <v>52.142857142857146</v>
       </c>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H63">
+    <row r="63" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M63">
         <v>6793</v>
       </c>
-      <c r="I63">
+      <c r="N63">
         <v>52.142857142857146</v>
       </c>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H64">
+    <row r="64" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M64">
         <v>6817</v>
       </c>
-      <c r="I64">
+      <c r="N64">
         <v>52.142857142857146</v>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H65">
+    <row r="65" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M65">
         <v>6841</v>
       </c>
-      <c r="I65">
+      <c r="N65">
         <v>52.142857142857146</v>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H66">
+    <row r="66" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M66">
         <v>6865</v>
       </c>
-      <c r="I66">
+      <c r="N66">
         <v>52.142857142857146</v>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H67">
+    <row r="67" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M67">
         <v>7225</v>
       </c>
-      <c r="I67">
+      <c r="N67">
         <v>4.7326870779999997</v>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H68">
-        <f t="shared" ref="H68:H73" si="8">H67+24</f>
+    <row r="68" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M68">
+        <f t="shared" ref="M68:M73" si="8">M67+24</f>
         <v>7249</v>
       </c>
-      <c r="I68">
+      <c r="N68">
         <v>4.7326870779999997</v>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H69">
+    <row r="69" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M69">
         <f t="shared" si="8"/>
         <v>7273</v>
       </c>
-      <c r="I69">
+      <c r="N69">
         <v>4.7326870779999997</v>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H70">
+    <row r="70" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M70">
         <f t="shared" si="8"/>
         <v>7297</v>
       </c>
-      <c r="I70">
+      <c r="N70">
         <v>4.7326870779999997</v>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H71">
+    <row r="71" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M71">
         <f t="shared" si="8"/>
         <v>7321</v>
       </c>
-      <c r="I71">
+      <c r="N71">
         <v>4.7326870779999997</v>
       </c>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H72">
+    <row r="72" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M72">
         <f t="shared" si="8"/>
         <v>7345</v>
       </c>
-      <c r="I72">
+      <c r="N72">
         <v>4.7326870779999997</v>
       </c>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H73">
+    <row r="73" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M73">
         <f t="shared" si="8"/>
         <v>7369</v>
       </c>
-      <c r="I73">
+      <c r="N73">
         <v>4.7326870779999997</v>
       </c>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H74">
+    <row r="74" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M74">
         <v>7897</v>
       </c>
-      <c r="I74">
+      <c r="N74">
         <v>4.6046707500000004</v>
       </c>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H75">
-        <f t="shared" ref="H75:H80" si="9">H74+24</f>
+    <row r="75" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M75">
+        <f t="shared" ref="M75:M80" si="9">M74+24</f>
         <v>7921</v>
       </c>
-      <c r="I75">
+      <c r="N75">
         <v>4.6046707500000004</v>
       </c>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H76">
+    <row r="76" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M76">
         <f t="shared" si="9"/>
         <v>7945</v>
       </c>
-      <c r="I76">
+      <c r="N76">
         <v>4.6046707500000004</v>
       </c>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H77">
+    <row r="77" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M77">
         <f t="shared" si="9"/>
         <v>7969</v>
       </c>
-      <c r="I77">
+      <c r="N77">
         <v>4.6046707500000004</v>
       </c>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H78">
+    <row r="78" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M78">
         <f t="shared" si="9"/>
         <v>7993</v>
       </c>
-      <c r="I78">
+      <c r="N78">
         <v>4.6046707500000004</v>
       </c>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H79">
+    <row r="79" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M79">
         <f t="shared" si="9"/>
         <v>8017</v>
       </c>
-      <c r="I79">
+      <c r="N79">
         <v>4.6046707500000004</v>
       </c>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H80">
+    <row r="80" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M80">
         <f t="shared" si="9"/>
         <v>8041</v>
       </c>
-      <c r="I80">
+      <c r="N80">
         <v>4.6046707500000004</v>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H81">
+    <row r="81" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M81">
         <v>8065</v>
       </c>
-      <c r="I81">
+      <c r="N81">
         <v>6.1457110019999996</v>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H82">
-        <f t="shared" ref="H82:H87" si="10">H81+24</f>
+    <row r="82" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M82">
+        <f t="shared" ref="M82:M87" si="10">M81+24</f>
         <v>8089</v>
       </c>
-      <c r="I82">
+      <c r="N82">
         <v>6.1457110019999996</v>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H83">
+    <row r="83" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M83">
         <f t="shared" si="10"/>
         <v>8113</v>
       </c>
-      <c r="I83">
+      <c r="N83">
         <v>6.1457110019999996</v>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H84">
+    <row r="84" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M84">
         <f t="shared" si="10"/>
         <v>8137</v>
       </c>
-      <c r="I84">
+      <c r="N84">
         <v>6.1457110019999996</v>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H85">
+    <row r="85" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M85">
         <f t="shared" si="10"/>
         <v>8161</v>
       </c>
-      <c r="I85">
+      <c r="N85">
         <v>6.1457110019999996</v>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H86">
+    <row r="86" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M86">
         <f t="shared" si="10"/>
         <v>8185</v>
       </c>
-      <c r="I86">
+      <c r="N86">
         <v>6.1457110019999996</v>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H87">
+    <row r="87" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M87">
         <f t="shared" si="10"/>
         <v>8209</v>
       </c>
-      <c r="I87">
+      <c r="N87">
         <v>6.1457110019999996</v>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H88">
+    <row r="88" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M88">
         <v>8401</v>
       </c>
-      <c r="I88">
+      <c r="N88">
         <v>2.9553183180000002</v>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H89">
-        <f t="shared" ref="H89:H94" si="11">H88+24</f>
+    <row r="89" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M89">
+        <f t="shared" ref="M89:M94" si="11">M88+24</f>
         <v>8425</v>
       </c>
-      <c r="I89">
+      <c r="N89">
         <v>2.9553183180000002</v>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H90">
+    <row r="90" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M90">
         <f t="shared" si="11"/>
         <v>8449</v>
       </c>
-      <c r="I90">
+      <c r="N90">
         <v>2.9553183180000002</v>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H91">
+    <row r="91" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M91">
         <f t="shared" si="11"/>
         <v>8473</v>
       </c>
-      <c r="I91">
+      <c r="N91">
         <v>2.9553183180000002</v>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H92">
+    <row r="92" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M92">
         <f t="shared" si="11"/>
         <v>8497</v>
       </c>
-      <c r="I92">
+      <c r="N92">
         <v>2.9553183180000002</v>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H93">
+    <row r="93" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M93">
         <f t="shared" si="11"/>
         <v>8521</v>
       </c>
-      <c r="I93">
+      <c r="N93">
         <v>2.9553183180000002</v>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H94">
+    <row r="94" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M94">
         <f t="shared" si="11"/>
         <v>8545</v>
       </c>
-      <c r="I94">
+      <c r="N94">
         <v>2.9553183180000002</v>
       </c>
     </row>

</xml_diff>